<commit_message>
feat: add parameters for table style, alignment, and font style parsing; update README and .gitignore
</commit_message>
<xml_diff>
--- a/example/test.xlsx
+++ b/example/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiarong/typst-xml-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiarong/typst-xml-parser/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1770F18-B520-A44E-A71F-4454325F9A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311F368A-733D-5E4D-AE2E-CBA272316476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17480" xr2:uid="{4E67DFF0-040B-4B55-998D-A8CA92707F79}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,9 +89,67 @@
       <charset val="134"/>
     </font>
     <font>
+      <i/>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color rgb="FFC00000"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="7" tint="0.59999389629810485"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="9" tint="0.59999389629810485"/>
       <name val="Microsoft YaHei Light"/>
       <family val="2"/>
       <charset val="134"/>
@@ -186,23 +244,47 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -210,6 +292,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,7 +616,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -541,30 +629,30 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -572,12 +660,12 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="25" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
+      <c r="A4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14" t="s">
         <v>0</v>
       </c>
     </row>
@@ -585,20 +673,20 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="25" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -612,10 +700,10 @@
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="21">
       <c r="C8" s="1" t="s">

</xml_diff>

<commit_message>
feat: add serde and toml dependencies; enhance xlsx-parser with improved table parsing and alignment handling
</commit_message>
<xml_diff>
--- a/example/test.xlsx
+++ b/example/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiarong/typst-xml-parser/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311F368A-733D-5E4D-AE2E-CBA272316476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D030AD-1A97-924F-B789-7F9B34ADDAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17480" xr2:uid="{4E67DFF0-040B-4B55-998D-A8CA92707F79}"/>
+    <workbookView xWindow="8860" yWindow="9000" windowWidth="29400" windowHeight="17480" xr2:uid="{4E67DFF0-040B-4B55-998D-A8CA92707F79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,6 +263,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -292,12 +298,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,7 +616,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D7"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -634,13 +634,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="25" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -648,24 +648,24 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="25" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="25" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14" t="s">
+    <row r="4" spans="1:4" ht="98" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16" t="s">
         <v>0</v>
       </c>
     </row>
@@ -679,13 +679,13 @@
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" ht="25" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
@@ -700,10 +700,10 @@
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="21">
       <c r="C8" s="1" t="s">

</xml_diff>

<commit_message>
feat: enhance xlsx-parser to support border and background color parsing; update example.typ for improved demonstration
</commit_message>
<xml_diff>
--- a/example/test.xlsx
+++ b/example/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiarong/typst-xml-parser/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D030AD-1A97-924F-B789-7F9B34ADDAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6D335D-9A34-8B4C-B284-0B632627E2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="9000" windowWidth="29400" windowHeight="17480" xr2:uid="{4E67DFF0-040B-4B55-998D-A8CA92707F79}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17480" xr2:uid="{4E67DFF0-040B-4B55-998D-A8CA92707F79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,14 +82,6 @@
     </font>
     <font>
       <i/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Microsoft YaHei Light"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <i/>
       <sz val="36"/>
       <color theme="1"/>
       <name val="Microsoft YaHei Light"/>
@@ -98,13 +90,6 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Microsoft YaHei Light"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color theme="8" tint="-0.499984740745262"/>
       <name val="Microsoft YaHei Light"/>
       <family val="2"/>
@@ -154,13 +139,60 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="5" tint="0.79998168889431442"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Microsoft YaHei Light"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -213,10 +245,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -227,9 +259,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -244,59 +274,68 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -616,7 +655,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -629,30 +668,30 @@
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25" customHeight="1">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -660,33 +699,33 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="98" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16" t="s">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4" ht="25" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -694,16 +733,16 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="25" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="A7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" ht="21">
       <c r="C8" s="1" t="s">

</xml_diff>